<commit_message>
Trig Practice in progress
</commit_message>
<xml_diff>
--- a/AgentAdvent/DataFiles/Test.xlsx
+++ b/AgentAdvent/DataFiles/Test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pat\ProgrammingProjects\PersonalProjects\AgentAdvent\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emily\Documents\Programming_Projects\PersonalProjects\AgentAdvent\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Exclusions</t>
   </si>
   <si>
-    <t>Pat &amp; Em</t>
-  </si>
-  <si>
     <t>Bekah</t>
   </si>
   <si>
@@ -51,12 +48,66 @@
   </si>
   <si>
     <t>Links</t>
+  </si>
+  <si>
+    <t>Pat</t>
+  </si>
+  <si>
+    <t>Em</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Mom</t>
+  </si>
+  <si>
+    <t>Dad</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Dad,Jessie</t>
+  </si>
+  <si>
+    <t>Jessie,Kenny</t>
+  </si>
+  <si>
+    <t>Mom,Em</t>
+  </si>
+  <si>
+    <t>Jessie,Dad</t>
+  </si>
+  <si>
+    <t>Emily,Bekah</t>
+  </si>
+  <si>
+    <t>Bill,Mom</t>
+  </si>
+  <si>
+    <t>Dad,Jo</t>
+  </si>
+  <si>
+    <t>Jo,Jonathan,Chrissy</t>
+  </si>
+  <si>
+    <t>Mom,Pat</t>
+  </si>
+  <si>
+    <t>Chrissy,Bekah,Bill</t>
+  </si>
+  <si>
+    <t>Kenny,Pat,Jon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,25 +440,37 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -415,17 +478,98 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>